<commit_message>
Update pytests and add single molecule input
</commit_message>
<xml_diff>
--- a/molmetrics/data/test_mini_sdf/mini_test_library_qed.xlsx
+++ b/molmetrics/data/test_mini_sdf/mini_test_library_qed.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85cb32c1384fb64c/Documents/GitHub/molmetrics/molmetrics/data/test_mini_sdf/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_AAFBF71F6DA059E5C0362E08F66E86A490FBAAE6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75FD2D1F-DB4E-49A6-8BD3-1327036EB773}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-105" yWindow="5640" windowWidth="36435" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -106,7 +100,7 @@
     <t>C#CCCCCNC(=O)Nc1cc(C)ccn1</t>
   </si>
   <si>
-    <t>&lt;rdkit.Chem.rdchem.Mol object at 0x7fca936634c0&gt;</t>
+    <t>&lt;rdkit.Chem.rdchem.Mol object at 0x7f61ac80f4c0&gt;</t>
   </si>
   <si>
     <t>Disc-like</t>
@@ -115,7 +109,7 @@
     <t>C#CCCCCNC(=O)Nc1ccc(C)cn1</t>
   </si>
   <si>
-    <t>&lt;rdkit.Chem.rdchem.Mol object at 0x7fca93663610&gt;</t>
+    <t>&lt;rdkit.Chem.rdchem.Mol object at 0x7f61ac80f610&gt;</t>
   </si>
   <si>
     <t>Balanced</t>
@@ -127,7 +121,7 @@
     <t>C#CCCCCNC(=O)Nc1ccc(F)cn1</t>
   </si>
   <si>
-    <t>&lt;rdkit.Chem.rdchem.Mol object at 0x7fca936635a0&gt;</t>
+    <t>&lt;rdkit.Chem.rdchem.Mol object at 0x7f61ac80f5a0&gt;</t>
   </si>
   <si>
     <t>C18H22N2O4S</t>
@@ -136,7 +130,7 @@
     <t>C#CCOc1ccccc1CN(CC1CN(S(C)(=O)=O)C1)C(=O)C=C</t>
   </si>
   <si>
-    <t>&lt;rdkit.Chem.rdchem.Mol object at 0x7fca93663680&gt;</t>
+    <t>&lt;rdkit.Chem.rdchem.Mol object at 0x7f61ac80f680&gt;</t>
   </si>
   <si>
     <t>C21H23FN2O2</t>
@@ -145,14 +139,14 @@
     <t>C#CCC1(C(=O)NCc2ccc(CNC(=O)C=C)cc2F)CC=CCC1</t>
   </si>
   <si>
-    <t>&lt;rdkit.Chem.rdchem.Mol object at 0x7fca936636f0&gt;</t>
+    <t>&lt;rdkit.Chem.rdchem.Mol object at 0x7f61ac80f6f0&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,14 +183,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -217,13 +203,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -261,13 +241,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -305,13 +279,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -349,13 +317,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -393,13 +355,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -437,13 +393,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -481,13 +431,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -525,13 +469,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -569,13 +507,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -613,13 +545,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -657,13 +583,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -701,13 +621,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -745,13 +659,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -789,13 +697,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="15" name="Picture 14" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -833,13 +735,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="16" name="Picture 15" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -866,9 +762,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -906,7 +802,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -940,7 +836,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -975,10 +870,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1151,21 +1045,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="47.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1245,7 +1136,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="150" customHeight="1">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1256,13 +1147,13 @@
         <v>28</v>
       </c>
       <c r="G2">
-        <v>0.61504053871208308</v>
+        <v>0.6150405387120831</v>
       </c>
       <c r="H2">
         <v>136.154</v>
       </c>
       <c r="I2">
-        <v>0.95831999999999984</v>
+        <v>0.9583199999999998</v>
       </c>
       <c r="J2">
         <v>2</v>
@@ -1301,22 +1192,22 @@
         <v>0</v>
       </c>
       <c r="V2">
-        <v>0.14285714285714279</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="W2">
-        <v>38.660700000000013</v>
+        <v>38.66070000000001</v>
       </c>
       <c r="X2">
-        <v>0.30105665295732159</v>
+        <v>0.3010566529573216</v>
       </c>
       <c r="Y2">
-        <v>0.70383384043255182</v>
+        <v>0.7038338404325518</v>
       </c>
       <c r="Z2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="150" customHeight="1">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1327,13 +1218,13 @@
         <v>31</v>
       </c>
       <c r="G3">
-        <v>0.61504053871208308</v>
+        <v>0.6150405387120831</v>
       </c>
       <c r="H3">
         <v>136.154</v>
       </c>
       <c r="I3">
-        <v>0.95831999999999984</v>
+        <v>0.9583199999999998</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1372,22 +1263,22 @@
         <v>0</v>
       </c>
       <c r="V3">
-        <v>0.14285714285714279</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="W3">
-        <v>38.660700000000013</v>
+        <v>38.66070000000001</v>
       </c>
       <c r="X3">
-        <v>0.16188011090315929</v>
+        <v>0.1618801109031593</v>
       </c>
       <c r="Y3">
-        <v>0.84237779725191753</v>
+        <v>0.8423777972519175</v>
       </c>
       <c r="Z3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="150" customHeight="1">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1398,13 +1289,13 @@
         <v>35</v>
       </c>
       <c r="G4">
-        <v>0.61680177722937668</v>
+        <v>0.6168017772293767</v>
       </c>
       <c r="H4">
-        <v>140.11699999999999</v>
+        <v>140.117</v>
       </c>
       <c r="I4">
-        <v>0.78900000000000015</v>
+        <v>0.7890000000000001</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -1446,19 +1337,19 @@
         <v>0</v>
       </c>
       <c r="W4">
-        <v>33.881700000000002</v>
+        <v>33.8817</v>
       </c>
       <c r="X4">
-        <v>0.15433009606280601</v>
+        <v>0.154330096062806</v>
       </c>
       <c r="Y4">
-        <v>0.84566990405699816</v>
+        <v>0.8456699040569982</v>
       </c>
       <c r="Z4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="150" customHeight="1">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1469,13 +1360,13 @@
         <v>38</v>
       </c>
       <c r="G5">
-        <v>0.78521872625513223</v>
+        <v>0.7852187262551322</v>
       </c>
       <c r="H5">
-        <v>324.40200000000021</v>
+        <v>324.4020000000002</v>
       </c>
       <c r="I5">
-        <v>0.79819999999999958</v>
+        <v>0.7981999999999996</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -1484,7 +1375,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>77.920000000000016</v>
+        <v>77.92000000000002</v>
       </c>
       <c r="M5">
         <v>6</v>
@@ -1517,19 +1408,19 @@
         <v>0.4</v>
       </c>
       <c r="W5">
-        <v>83.627600000000029</v>
+        <v>83.62760000000003</v>
       </c>
       <c r="X5">
-        <v>0.32925542890277998</v>
+        <v>0.32925542890278</v>
       </c>
       <c r="Y5">
-        <v>0.74699082071287193</v>
+        <v>0.7469908207128719</v>
       </c>
       <c r="Z5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="150" customHeight="1">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1540,10 +1431,10 @@
         <v>41</v>
       </c>
       <c r="G6">
-        <v>0.62591443190941443</v>
+        <v>0.6259144319094144</v>
       </c>
       <c r="H6">
-        <v>316.37600000000009</v>
+        <v>316.3760000000001</v>
       </c>
       <c r="I6">
         <v>2.6004</v>
@@ -1585,16 +1476,16 @@
         <v>0</v>
       </c>
       <c r="V6">
-        <v>0.33333333333333331</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="W6">
-        <v>86.771400000000042</v>
+        <v>86.77140000000004</v>
       </c>
       <c r="X6">
-        <v>0.18023813896922161</v>
+        <v>0.1802381389692216</v>
       </c>
       <c r="Y6">
-        <v>0.93463460843248014</v>
+        <v>0.9346346084324801</v>
       </c>
       <c r="Z6" t="s">
         <v>32</v>

</xml_diff>